<commit_message>
Added the sales order test cases
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Downloads\X4A_Auto_updated\X4A_Auto_New\X4A_Auto\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\X4A\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1FB187-6C4E-4F8B-86BF-9749138612ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329E989B-8CA3-416A-ABE8-16055349C2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2370" windowWidth="25830" windowHeight="11685" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="0" yWindow="2310" windowWidth="25830" windowHeight="11685" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -47,10 +47,37 @@
     <t>ResellerBCN</t>
   </si>
   <si>
-    <t>sales_order</t>
-  </si>
-  <si>
     <t>aged_orders</t>
+  </si>
+  <si>
+    <t>sales_orders</t>
+  </si>
+  <si>
+    <t>IMOrderNo</t>
+  </si>
+  <si>
+    <t>20-RP39N-11</t>
+  </si>
+  <si>
+    <t>OrderType</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>VendorName</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>PO12345</t>
+  </si>
+  <si>
+    <t>MICROSOFT HARDWARE</t>
+  </si>
+  <si>
+    <t>Order Hold</t>
   </si>
 </sst>
 </file>
@@ -75,6 +102,7 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -126,11 +154,11 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,50 +473,74 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="4">
+        <v>20222222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B3" s="4">
         <v>20222222</v>
       </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
-        <v>20222222</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aged order validation code added
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Downloads\X4A_Auto_updated\X4A_Auto_New\X4A_Auto\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1FB187-6C4E-4F8B-86BF-9749138612ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478190C7-1BEF-4282-B5D1-31689F50CC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2370" windowWidth="25830" windowHeight="11685" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="1710" yWindow="2025" windowWidth="14025" windowHeight="5895" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,28 +36,85 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FeatureFileName</t>
   </si>
   <si>
+    <t>ResellerBCN</t>
+  </si>
+  <si>
+    <t>IMOrderNo</t>
+  </si>
+  <si>
+    <t>OrderType</t>
+  </si>
+  <si>
     <t>ResellerPO</t>
   </si>
   <si>
-    <t>ResellerBCN</t>
-  </si>
-  <si>
-    <t>sales_order</t>
+    <t>VendorName</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
   </si>
   <si>
     <t>aged_orders</t>
+  </si>
+  <si>
+    <t>sales_orders</t>
+  </si>
+  <si>
+    <t>20-RP39N-11</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>PO12345</t>
+  </si>
+  <si>
+    <t>MICROSOFT HARDWARE</t>
+  </si>
+  <si>
+    <t>Order Hold</t>
+  </si>
+  <si>
+    <t>20-RGHD8-11</t>
+  </si>
+  <si>
+    <t>WDT - RETAIL FLASH USB</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>Direct</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>CustomerPO</t>
+  </si>
+  <si>
+    <t>TotalRevenueMin</t>
+  </si>
+  <si>
+    <t>TotalRevenueMax</t>
+  </si>
+  <si>
+    <t>EPLUS TECHNOLOGY INC</t>
+  </si>
+  <si>
+    <t>CustomerName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -70,6 +127,12 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -123,14 +186,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,51 +511,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="25.140625" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
+    <col min="9" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>1</v>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="4">
         <v>20222222</v>
       </c>
-      <c r="C2">
-        <v>1</v>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>400</v>
+      </c>
+      <c r="K2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4">
         <v>20222222</v>
       </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C5" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated data for aged orders
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{478190C7-1BEF-4282-B5D1-31689F50CC66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2F2E9-CED8-41EE-B855-815E78E39F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1710" yWindow="2025" windowWidth="14025" windowHeight="5895" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -83,9 +83,6 @@
     <t>20-RGHD8-11</t>
   </si>
   <si>
-    <t>WDT - RETAIL FLASH USB</t>
-  </si>
-  <si>
     <t>TEST</t>
   </si>
   <si>
@@ -108,6 +105,12 @@
   </si>
   <si>
     <t>CustomerName</t>
+  </si>
+  <si>
+    <t>STARTECH.COM</t>
+  </si>
+  <si>
+    <t>APPLE MINI IPADS</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -553,16 +556,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
-      </c>
       <c r="K1" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -570,22 +573,22 @@
         <v>7</v>
       </c>
       <c r="B2" s="4">
-        <v>20222222</v>
+        <v>30036215</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" t="s">
-        <v>16</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -594,7 +597,7 @@
         <v>400</v>
       </c>
       <c r="K2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -622,6 +625,14 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
+        <v>60588621</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated aged order details
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E2F2E9-CED8-41EE-B855-815E78E39F3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7821FCE-077B-42CB-B0B6-F8327ACF7F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -105,9 +105,6 @@
   </si>
   <si>
     <t>CustomerName</t>
-  </si>
-  <si>
-    <t>STARTECH.COM</t>
   </si>
   <si>
     <t>APPLE MINI IPADS</t>
@@ -517,7 +514,7 @@
   <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,7 +579,7 @@
         <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -627,12 +624,7 @@
       <c r="C5" s="5"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
-        <v>60588621</v>
-      </c>
-      <c r="F8" t="s">
-        <v>23</v>
-      </c>
+      <c r="B8" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added the Sales Orders->Order Details Page test cases
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\X4A\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7821FCE-077B-42CB-B0B6-F8327ACF7F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C0525-51A6-4A39-AD86-9152C4A3F9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="0" yWindow="2055" windowWidth="25665" windowHeight="11340" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -65,21 +65,12 @@
     <t>sales_orders</t>
   </si>
   <si>
-    <t>20-RP39N-11</t>
-  </si>
-  <si>
-    <t>Stock</t>
-  </si>
-  <si>
     <t>PO12345</t>
   </si>
   <si>
     <t>MICROSOFT HARDWARE</t>
   </si>
   <si>
-    <t>Order Hold</t>
-  </si>
-  <si>
     <t>20-RGHD8-11</t>
   </si>
   <si>
@@ -108,13 +99,70 @@
   </si>
   <si>
     <t>APPLE MINI IPADS</t>
+  </si>
+  <si>
+    <t>OrderValue</t>
+  </si>
+  <si>
+    <t>ReferenceNumbers</t>
+  </si>
+  <si>
+    <t>BillingToInfo</t>
+  </si>
+  <si>
+    <t>ShipToInfo</t>
+  </si>
+  <si>
+    <t>EndUserInfo</t>
+  </si>
+  <si>
+    <t>OrderLinesTab</t>
+  </si>
+  <si>
+    <t>SerialNumbers</t>
+  </si>
+  <si>
+    <t>AdditionalAttributes</t>
+  </si>
+  <si>
+    <t>.,.,.,.,.,.</t>
+  </si>
+  <si>
+    <t>009,BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,5</t>
+  </si>
+  <si>
+    <t>0,0,S</t>
+  </si>
+  <si>
+    <t>50-ZBBZG-21</t>
+  </si>
+  <si>
+    <t>Order Hold(IM)</t>
+  </si>
+  <si>
+    <t>.,5B2MCF8007,.,.</t>
+  </si>
+  <si>
+    <t>0,AMAZON.COM SERVICES INC,PO BOX 80387 AMAZON.COM SEATTLE WA 981081309 US,.,.,.</t>
+  </si>
+  <si>
+    <t>200,AMAZON.COM,1600 NEWLANDS DR E FERNLEY NV 894088903 FERNLEY NV 894088903,.,.,.,.</t>
+  </si>
+  <si>
+    <t>009,Order Hold(IM),BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,.,322.28,1611.4,300,1500,6.91,USD,5,5,0,.</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -138,6 +186,13 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -186,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -196,6 +251,11 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -511,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -524,13 +584,21 @@
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="5" width="14.42578125" customWidth="1"/>
     <col min="6" max="6" width="25.140625" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="23.5703125" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="34.28515625" customWidth="1"/>
+    <col min="14" max="14" width="81.5703125" customWidth="1"/>
+    <col min="15" max="15" width="69.140625" customWidth="1"/>
+    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="126.140625" customWidth="1"/>
+    <col min="18" max="18" width="77.85546875" customWidth="1"/>
+    <col min="19" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,19 +621,43 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="N1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -573,19 +665,19 @@
         <v>30036215</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
       <c r="H2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -594,10 +686,10 @@
         <v>400</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -605,25 +697,49 @@
         <v>20222222</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="F3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>33</v>
+      </c>
+      <c r="L3" s="6">
+        <v>1793.58</v>
+      </c>
+      <c r="M3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>30</v>
+      </c>
+      <c r="S3" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="C5" s="5"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Beta data for sales and aged orders
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\X4A\x4a-automation-test-suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{951C0525-51A6-4A39-AD86-9152C4A3F9C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7354F6F9-7B47-4560-96A2-6AA67D2F159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2055" windowWidth="25665" windowHeight="11340" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -71,18 +71,6 @@
     <t>MICROSOFT HARDWARE</t>
   </si>
   <si>
-    <t>20-RGHD8-11</t>
-  </si>
-  <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Direct</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
     <t>CustomerPO</t>
   </si>
   <si>
@@ -92,15 +80,9 @@
     <t>TotalRevenueMax</t>
   </si>
   <si>
-    <t>EPLUS TECHNOLOGY INC</t>
-  </si>
-  <si>
     <t>CustomerName</t>
   </si>
   <si>
-    <t>APPLE MINI IPADS</t>
-  </si>
-  <si>
     <t>OrderValue</t>
   </si>
   <si>
@@ -134,9 +116,6 @@
     <t>0,0,S</t>
   </si>
   <si>
-    <t>50-ZBBZG-21</t>
-  </si>
-  <si>
     <t>Order Hold(IM)</t>
   </si>
   <si>
@@ -153,6 +132,27 @@
   </si>
   <si>
     <t>S</t>
+  </si>
+  <si>
+    <t>20-VK5Q2-11</t>
+  </si>
+  <si>
+    <t>Stock</t>
+  </si>
+  <si>
+    <t>PLANTRONICS-SPECIAL</t>
+  </si>
+  <si>
+    <t>Order Hold</t>
+  </si>
+  <si>
+    <t>DELL MARKETING LP</t>
+  </si>
+  <si>
+    <t>6057590163844402</t>
+  </si>
+  <si>
+    <t>20-VN1CR-11</t>
   </si>
 </sst>
 </file>
@@ -162,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -194,6 +194,18 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -203,7 +215,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -237,11 +249,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFEEEEEE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -257,6 +278,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -574,7 +607,7 @@
   <dimension ref="A1:S8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,63 +654,63 @@
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="O1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="Q1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="7" t="s">
+      <c r="S1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>28</v>
-      </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
-        <v>30036215</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>11</v>
+      <c r="B2" s="12">
+        <v>20036212</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -685,8 +718,8 @@
       <c r="J2">
         <v>400</v>
       </c>
-      <c r="K2" t="s">
-        <v>18</v>
+      <c r="K2" s="11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
@@ -697,10 +730,10 @@
         <v>20222222</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -709,35 +742,43 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="L3" s="6">
         <v>1793.58</v>
       </c>
       <c r="M3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="Q3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="R3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="S3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="C5" s="5"/>
+    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="9"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="H5" s="10"/>
+      <c r="K5" s="10"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>

</xml_diff>

<commit_message>
Added Fraud Reprocess and Cancel Order test cases
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7354F6F9-7B47-4560-96A2-6AA67D2F159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFEC3AA-C51E-468D-BBEA-7D7B48D6A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="20040" windowHeight="10230" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -153,6 +153,21 @@
   </si>
   <si>
     <t>20-VN1CR-11</t>
+  </si>
+  <si>
+    <t>fraud_orders</t>
+  </si>
+  <si>
+    <t>FraudCancelOrderConfirmationId</t>
+  </si>
+  <si>
+    <t>FraudReprocessOrderConfirmationId</t>
+  </si>
+  <si>
+    <t>US-C-23080455071226315254</t>
+  </si>
+  <si>
+    <t>US-C-23080226523476649177</t>
   </si>
 </sst>
 </file>
@@ -604,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:U8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,9 +644,11 @@
     <col min="17" max="17" width="126.140625" customWidth="1"/>
     <col min="18" max="18" width="77.85546875" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
+    <col min="20" max="20" width="32.28515625" customWidth="1"/>
+    <col min="21" max="21" width="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,8 +706,14 @@
       <c r="S1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="T1" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -722,7 +745,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -769,18 +792,29 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T4" t="s">
+        <v>42</v>
+      </c>
+      <c r="U4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reseller name column added
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7354F6F9-7B47-4560-96A2-6AA67D2F159E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270DF569-A20A-4629-9191-235F1224D19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -131,12 +131,6 @@
     <t>009,Order Hold(IM),BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,.,322.28,1611.4,300,1500,6.91,USD,5,5,0,.</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>20-VK5Q2-11</t>
-  </si>
-  <si>
     <t>Stock</t>
   </si>
   <si>
@@ -153,6 +147,24 @@
   </si>
   <si>
     <t>20-VN1CR-11</t>
+  </si>
+  <si>
+    <t>50-74321-11</t>
+  </si>
+  <si>
+    <t>41-22244-14</t>
+  </si>
+  <si>
+    <t>41-64551-11</t>
+  </si>
+  <si>
+    <t>37-26283-11</t>
+  </si>
+  <si>
+    <t>APPLE</t>
+  </si>
+  <si>
+    <t>ResellerName</t>
   </si>
 </sst>
 </file>
@@ -162,7 +174,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,6 +217,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF172B4D"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -262,7 +280,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -290,6 +308,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,10 +623,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -631,7 +650,7 @@
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,28 +708,31 @@
       <c r="S1" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="T1" s="7" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="12">
         <v>20036212</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -719,10 +741,10 @@
         <v>400</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -730,7 +752,7 @@
         <v>20222222</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -768,20 +790,40 @@
       <c r="S3" t="s">
         <v>25</v>
       </c>
+      <c r="T3" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:19" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="17.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E6" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
+      <c r="E7" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="4">
+        <v>20222222</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added Data Error Orders test case
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFEC3AA-C51E-468D-BBEA-7D7B48D6A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D48E46E-3C06-42EA-A975-1A3796BBBB8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1950" yWindow="1950" windowWidth="20040" windowHeight="10230" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>US-C-23080226523476649177</t>
+  </si>
+  <si>
+    <t>data_errors_orders</t>
+  </si>
+  <si>
+    <t>DataErrorResubmitOrderConfirmationId</t>
   </si>
 </sst>
 </file>
@@ -619,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:V8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -645,10 +651,11 @@
     <col min="18" max="18" width="77.85546875" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
     <col min="20" max="20" width="32.28515625" customWidth="1"/>
-    <col min="21" max="21" width="32" customWidth="1"/>
+    <col min="21" max="21" width="35.42578125" customWidth="1"/>
+    <col min="22" max="22" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -712,8 +719,11 @@
       <c r="U1" s="7" t="s">
         <v>41</v>
       </c>
+      <c r="V1" s="7" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -745,7 +755,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:22" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -792,7 +802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>39</v>
       </c>
@@ -803,18 +813,21 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Filter testcases for sales order added
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFEC3AA-C51E-468D-BBEA-7D7B48D6A152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A9D9DB-C117-4440-9849-41F17E5E7822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="20040" windowHeight="10230" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -116,9 +116,6 @@
     <t>0,0,S</t>
   </si>
   <si>
-    <t>Order Hold(IM)</t>
-  </si>
-  <si>
     <t>.,5B2MCF8007,.,.</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>009,Order Hold(IM),BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,.,322.28,1611.4,300,1500,6.91,USD,5,5,0,.</t>
   </si>
   <si>
-    <t>S</t>
-  </si>
-  <si>
     <t>20-VK5Q2-11</t>
   </si>
   <si>
@@ -168,6 +162,27 @@
   </si>
   <si>
     <t>US-C-23080226523476649177</t>
+  </si>
+  <si>
+    <t>ResellerName</t>
+  </si>
+  <si>
+    <t>EndUserName</t>
+  </si>
+  <si>
+    <t>Everest EndUser</t>
+  </si>
+  <si>
+    <t>CreatedOn</t>
+  </si>
+  <si>
+    <t>Yesterday</t>
+  </si>
+  <si>
+    <t>INGRAM MICRO CAP TEST ACCOUNT</t>
+  </si>
+  <si>
+    <t>20-VN2W9-11</t>
   </si>
 </sst>
 </file>
@@ -619,10 +634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:U8"/>
+  <dimension ref="A1:X9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,9 +661,11 @@
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
     <col min="20" max="20" width="32.28515625" customWidth="1"/>
     <col min="21" max="21" width="32" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -707,13 +724,22 @@
         <v>22</v>
       </c>
       <c r="T1" s="7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="U1" s="7" t="s">
-        <v>41</v>
+        <v>39</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -721,19 +747,19 @@
         <v>20036212</v>
       </c>
       <c r="C2" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="14" t="s">
         <v>35</v>
-      </c>
-      <c r="H2" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -742,10 +768,10 @@
         <v>400</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -753,7 +779,7 @@
         <v>20222222</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -765,25 +791,31 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>300</v>
       </c>
       <c r="L3" s="6">
         <v>1793.58</v>
       </c>
       <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
         <v>27</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" s="8" t="s">
         <v>28</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>29</v>
       </c>
       <c r="P3" t="s">
         <v>23</v>
       </c>
       <c r="Q3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R3" t="s">
         <v>24</v>
@@ -791,31 +823,45 @@
       <c r="S3" t="s">
         <v>25</v>
       </c>
+      <c r="V3" t="s">
+        <v>47</v>
+      </c>
+      <c r="W3" t="s">
+        <v>44</v>
+      </c>
+      <c r="X3" t="s">
+        <v>46</v>
+      </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="T4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="U4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
end user po column added
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A313442-E518-46C7-9240-516DDCDC0EBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E3480C-D03A-4004-A190-72EC7B177AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -197,7 +197,16 @@
     <t>FilterOrderStatus</t>
   </si>
   <si>
-    <t>20-VN2W9-11</t>
+    <t>37-26283-11</t>
+  </si>
+  <si>
+    <t>abc</t>
+  </si>
+  <si>
+    <t>EndUserPO</t>
+  </si>
+  <si>
+    <t>EPO123</t>
   </si>
 </sst>
 </file>
@@ -649,10 +658,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,7 +688,7 @@
     <col min="22" max="22" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -761,8 +770,11 @@
       <c r="AA1" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="AC1" s="7" t="s">
+        <v>55</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -794,7 +806,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -816,6 +828,9 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
       <c r="I3">
         <v>0</v>
       </c>
@@ -861,8 +876,11 @@
       <c r="AA3" t="s">
         <v>35</v>
       </c>
+      <c r="AC3" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
@@ -873,7 +891,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -883,11 +901,11 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sales order edit tcs added
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E3480C-D03A-4004-A190-72EC7B177AE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40155E8-4E48-460E-9F22-3D46A5630D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="60">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -207,6 +207,15 @@
   </si>
   <si>
     <t>EPO123</t>
+  </si>
+  <si>
+    <t>20-32122-11</t>
+  </si>
+  <si>
+    <t>EditOrderLines</t>
+  </si>
+  <si>
+    <t>20,60,3</t>
   </si>
 </sst>
 </file>
@@ -216,7 +225,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,6 +268,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF333333"/>
+      <name val="Roboto"/>
     </font>
   </fonts>
   <fills count="2">
@@ -316,7 +331,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -344,6 +359,15 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,10 +682,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AC8"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AA11" sqref="AA11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -683,9 +707,9 @@
     <col min="17" max="17" width="126.140625" customWidth="1"/>
     <col min="18" max="18" width="77.85546875" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
-    <col min="20" max="20" width="32.28515625" customWidth="1"/>
-    <col min="21" max="21" width="35.42578125" customWidth="1"/>
-    <col min="22" max="22" width="26.85546875" customWidth="1"/>
+    <col min="20" max="20" width="27.140625" customWidth="1"/>
+    <col min="21" max="21" width="29" customWidth="1"/>
+    <col min="22" max="22" width="9.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.25">
@@ -770,8 +794,11 @@
       <c r="AA1" s="7" t="s">
         <v>52</v>
       </c>
+      <c r="AB1" s="7" t="s">
+        <v>55</v>
+      </c>
       <c r="AC1" s="7" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -806,15 +833,15 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="4">
         <v>20222222</v>
       </c>
-      <c r="C3" t="s">
-        <v>53</v>
+      <c r="C3" s="17" t="s">
+        <v>57</v>
       </c>
       <c r="D3" t="s">
         <v>31</v>
@@ -876,8 +903,11 @@
       <c r="AA3" t="s">
         <v>35</v>
       </c>
+      <c r="AB3" t="s">
+        <v>56</v>
+      </c>
       <c r="AC3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:29" x14ac:dyDescent="0.25">
@@ -900,6 +930,9 @@
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
@@ -908,6 +941,14 @@
     <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
+    <row r="10" spans="1:29" ht="46.5" x14ac:dyDescent="0.25">
+      <c r="B10" s="15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Modify Reference Details, shipping Notes and Filters  test case
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D85ABD-BA62-452E-B211-0E892E5FEFD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5090F23C-7304-40B5-883F-C9B28DD23D2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="3855" yWindow="1350" windowWidth="22200" windowHeight="10230" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="59">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -107,9 +107,6 @@
     <t>AdditionalAttributes</t>
   </si>
   <si>
-    <t>.,.,.,.,.,.</t>
-  </si>
-  <si>
     <t>009,BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,5</t>
   </si>
   <si>
@@ -119,15 +116,6 @@
     <t>Order Hold(IM)</t>
   </si>
   <si>
-    <t>.,5B2MCF8007,.,.</t>
-  </si>
-  <si>
-    <t>0,AMAZON.COM SERVICES INC,PO BOX 80387 AMAZON.COM SEATTLE WA 981081309 US,.,.,.</t>
-  </si>
-  <si>
-    <t>200,AMAZON.COM,1600 NEWLANDS DR E FERNLEY NV 894088903 FERNLEY NV 894088903,.,.,.,.</t>
-  </si>
-  <si>
     <t>009,Order Hold(IM),BE43T-H 43IN BET SERIES COMM TV CRYSTAL UHD 250NIT 16/7 YRS,BE43T-H,7LN861,.,322.28,1611.4,300,1500,6.91,USD,5,5,0,.</t>
   </si>
   <si>
@@ -152,12 +140,6 @@
     <t>FraudReprocessOrderConfirmationId</t>
   </si>
   <si>
-    <t>US-C-23080455071226315254</t>
-  </si>
-  <si>
-    <t>US-C-23080226523476649177</t>
-  </si>
-  <si>
     <t>data_errors_orders</t>
   </si>
   <si>
@@ -188,9 +170,6 @@
     <t>FilterOrderStatus</t>
   </si>
   <si>
-    <t>20-VN2W9-11</t>
-  </si>
-  <si>
     <t>50-74803-22</t>
   </si>
   <si>
@@ -201,6 +180,39 @@
   </si>
   <si>
     <t>In Progress</t>
+  </si>
+  <si>
+    <t>ModifyReferenceDetailsDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>ModifyShippingNotesDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>ModifyVMFDetailsDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>ModifyEndUserDetailsDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>0,INGRAM MICRO CAP TEST ACCOUNT,1759 WEHRLE DR TEST WILLIAMSVILLE NY 142217033 US,.,.,.</t>
+  </si>
+  <si>
+    <t>200,INGRAM MICRO TEST ACCOUNT,ATTN TOD DEBIE 1610 E SAINT ANDREW PL SANTA ANA CA 927054931 SANTA ANA CA 927054931,.,.,.,.</t>
+  </si>
+  <si>
+    <t>.,AASHIK HOSPITALS,201 W GRAND BLVD CHEEKTOWAGA NY 142253017 US,.,.,.</t>
+  </si>
+  <si>
+    <t>20-VN9MH-21</t>
+  </si>
+  <si>
+    <t>.,RESE1A2SSS45,.,.</t>
+  </si>
+  <si>
+    <t>US-C-23090155303948313467</t>
+  </si>
+  <si>
+    <t>US-C-23083146274630246347</t>
   </si>
 </sst>
 </file>
@@ -649,10 +661,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AA8"/>
+  <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E39" workbookViewId="0">
-      <selection activeCell="L60" sqref="L60"/>
+    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,18 +680,23 @@
     <col min="11" max="11" width="23.5703125" customWidth="1"/>
     <col min="12" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="13" width="34.28515625" customWidth="1"/>
-    <col min="14" max="14" width="81.5703125" customWidth="1"/>
-    <col min="15" max="15" width="69.140625" customWidth="1"/>
-    <col min="16" max="16" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="85.5703125" customWidth="1"/>
+    <col min="15" max="15" width="115.28515625" customWidth="1"/>
+    <col min="16" max="16" width="73.5703125" customWidth="1"/>
     <col min="17" max="17" width="126.140625" customWidth="1"/>
-    <col min="18" max="18" width="77.85546875" customWidth="1"/>
+    <col min="18" max="18" width="77.5703125" customWidth="1"/>
     <col min="19" max="19" width="20.7109375" customWidth="1"/>
     <col min="20" max="20" width="32.28515625" customWidth="1"/>
     <col min="21" max="21" width="35.42578125" customWidth="1"/>
     <col min="22" max="22" width="26.85546875" customWidth="1"/>
+    <col min="27" max="27" width="22.85546875" customWidth="1"/>
+    <col min="28" max="28" width="40.42578125" customWidth="1"/>
+    <col min="29" max="29" width="35.85546875" customWidth="1"/>
+    <col min="30" max="30" width="34.85546875" customWidth="1"/>
+    <col min="31" max="31" width="35.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -738,31 +755,43 @@
         <v>22</v>
       </c>
       <c r="T1" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="U1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="W1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="AA1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z1" s="7" t="s">
+      <c r="AB1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="AA1" s="7" t="s">
+      <c r="AC1" s="7" t="s">
         <v>49</v>
       </c>
+      <c r="AD1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="AE1" s="7" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -770,19 +799,19 @@
         <v>20222222</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -791,10 +820,10 @@
         <v>400</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -802,10 +831,10 @@
         <v>20222222</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
@@ -814,7 +843,7 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -823,59 +852,59 @@
         <v>400</v>
       </c>
       <c r="L3" s="6">
-        <v>1793.58</v>
+        <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>56</v>
       </c>
       <c r="N3" t="s">
+        <v>52</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="P3" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R3" t="s">
+        <v>23</v>
+      </c>
+      <c r="S3" t="s">
+        <v>24</v>
+      </c>
+      <c r="W3" t="s">
+        <v>39</v>
+      </c>
+      <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z3" t="s">
         <v>28</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="AA3" t="s">
         <v>29</v>
       </c>
-      <c r="P3" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" t="s">
-        <v>25</v>
-      </c>
-      <c r="W3" t="s">
-        <v>45</v>
-      </c>
-      <c r="X3" t="s">
-        <v>46</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>33</v>
-      </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="T4" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="U4" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
@@ -883,11 +912,11 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UI automation to cancel single line item
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingrammicro-my.sharepoint.com/personal/shubhamg_deshmukh_ingrammicro_com/Documents/Documents/GitHub/shubham-x4a-automation-test-suite/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{994D9B72-7E7B-41EB-B2C4-6E40AD9D59B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{994D9B72-7E7B-41EB-B2C4-6E40AD9D59B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95E1391C-95B7-47DB-AB3A-3BA875E73345}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <t>20,60,3</t>
   </si>
   <si>
-    <t>20-RPHQ0-11</t>
+    <t>20-VNF3C-11</t>
   </si>
 </sst>
 </file>
@@ -377,6 +377,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -678,9 +682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
   <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Added Modify End User and and Billing address test cases
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingrammicro-my.sharepoint.com/personal/shubhamg_deshmukh_ingrammicro_com/Documents/Documents/GitHub/shubham-x4a-automation-test-suite/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{994D9B72-7E7B-41EB-B2C4-6E40AD9D59B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95E1391C-95B7-47DB-AB3A-3BA875E73345}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D25BFC5-BA8F-4615-ADFE-5FF326768B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="4260" yWindow="6555" windowWidth="22200" windowHeight="6825" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -225,6 +225,9 @@
   </si>
   <si>
     <t>20-VNF3C-11</t>
+  </si>
+  <si>
+    <t>ModifyBillingAddressDataErrorOrderID</t>
   </si>
 </sst>
 </file>
@@ -377,10 +380,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -680,9 +679,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AG8"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AF6" sqref="AF6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -711,9 +712,12 @@
     <col min="29" max="29" width="35.85546875" customWidth="1"/>
     <col min="30" max="30" width="34.85546875" customWidth="1"/>
     <col min="31" max="31" width="35.28515625" customWidth="1"/>
+    <col min="32" max="32" width="17.140625" customWidth="1"/>
+    <col min="33" max="33" width="18" customWidth="1"/>
+    <col min="34" max="34" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -813,8 +817,11 @@
       <c r="AG1" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="AH1" s="7" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -846,7 +853,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -920,7 +927,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -931,7 +938,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -941,11 +948,11 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Billing Address column
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingrammicro-my.sharepoint.com/personal/shubhamg_deshmukh_ingrammicro_com/Documents/Documents/GitHub/shubham-x4a-automation-test-suite/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{994D9B72-7E7B-41EB-B2C4-6E40AD9D59B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3892A42B-EFF0-4B71-A4E0-0723F446B39A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D560F8-931E-4431-A5A1-098645422D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="22200" windowHeight="6825" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>20-VNF4J-11</t>
+  </si>
+  <si>
+    <t>ModifyBillingAddressDataErrorOrderID</t>
   </si>
 </sst>
 </file>
@@ -383,10 +386,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -686,9 +685,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AG8"/>
+  <dimension ref="A1:AH8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AI5" sqref="AI5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -721,7 +722,7 @@
     <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -821,8 +822,11 @@
       <c r="AG1" s="7" t="s">
         <v>59</v>
       </c>
+      <c r="AH1" s="7" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -854,7 +858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -928,7 +932,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -939,7 +943,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:33" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -949,7 +953,7 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:33" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -1023,11 +1027,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Remove Exiting Line (OMS-29) test cases.
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7D560F8-931E-4431-A5A1-098645422D0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1E903F-A9AA-4923-A4EE-508CD0B3DC4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="2730" windowWidth="22200" windowHeight="6825" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="1575" yWindow="2730" windowWidth="24420" windowHeight="8010" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -227,13 +227,19 @@
     <t>sales_orders_edit</t>
   </si>
   <si>
-    <t>20-VNFJV-11</t>
-  </si>
-  <si>
     <t>20-VNF4J-11</t>
   </si>
   <si>
     <t>ModifyBillingAddressDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>20-VN9MH-21</t>
+  </si>
+  <si>
+    <t>200,INGRAM MICRO TEST ACCOUNT,ATTN TOD DEBIE 1610 E SAINT ANDREW PL SANTA ANA CA 927054931,.,.,.,.</t>
+  </si>
+  <si>
+    <t>OrderLineDataErrorOrderID</t>
   </si>
 </sst>
 </file>
@@ -685,10 +691,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AH8"/>
+  <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AI5" sqref="AI5"/>
+    <sheetView tabSelected="1" topLeftCell="AC1" workbookViewId="0">
+      <selection activeCell="AI6" sqref="AI6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,9 +726,12 @@
     <col min="30" max="30" width="34.85546875" customWidth="1"/>
     <col min="31" max="31" width="35.28515625" customWidth="1"/>
     <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36" customWidth="1"/>
+    <col min="35" max="35" width="22.5703125" customWidth="1"/>
+    <col min="36" max="36" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -823,10 +832,13 @@
         <v>59</v>
       </c>
       <c r="AH1" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="AI1" s="7" t="s">
+        <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -858,7 +870,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -866,7 +878,7 @@
         <v>20222222</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -896,7 +908,7 @@
         <v>52</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="P3" t="s">
         <v>54</v>
@@ -932,7 +944,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -943,7 +955,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -953,7 +965,7 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:34" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>62</v>
       </c>
@@ -961,7 +973,7 @@
         <v>20222222</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1027,11 +1039,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the Code for Filter and Update/Modify existing order line scenario.
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ingrammicro-my.sharepoint.com/personal/shubhamg_deshmukh_ingrammicro_com/Documents/Documents/GitHub/shubham-x4a-automation-test-suite/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{D4523A43-1156-4F7B-922B-B6DC52F3FED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{409DD8BC-0D47-4A54-A374-E95B9B96D7E0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C0906-6F95-44CB-B6A3-3F4BE4DF1DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="1575" yWindow="75" windowWidth="14745" windowHeight="10665" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -240,6 +240,9 @@
   </si>
   <si>
     <t>200,INGRAM MICRO TEST ACCOUNT,1610 E SAINT ANDREW PL ATTN TOD DEBIE SANTA ANA CA</t>
+  </si>
+  <si>
+    <t>ModifyOrderLineDataErrorOrderID</t>
   </si>
 </sst>
 </file>
@@ -392,10 +395,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -695,9 +694,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AI8"/>
+  <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AK9" sqref="AK9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -729,11 +730,11 @@
     <col min="31" max="31" width="35.28515625" customWidth="1"/>
     <col min="32" max="32" width="20.85546875" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="36" customWidth="1"/>
-    <col min="35" max="35" width="22.5703125" customWidth="1"/>
-    <col min="36" max="36" width="21" customWidth="1"/>
+    <col min="35" max="35" width="27.85546875" customWidth="1"/>
+    <col min="36" max="36" width="31.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -839,8 +840,11 @@
       <c r="AI1" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="AJ1" s="7" t="s">
+        <v>68</v>
+      </c>
     </row>
-    <row r="2" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -872,7 +876,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:35" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -946,7 +950,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -957,7 +961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -967,7 +971,7 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -1041,11 +1045,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated end user info for sales_order_edit
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C0906-6F95-44CB-B6A3-3F4BE4DF1DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D08433CE-B069-4B4F-819D-C591B91D1209}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="75" windowWidth="14745" windowHeight="10665" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="72">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -236,13 +236,22 @@
     <t>20-VLJ7K-31</t>
   </si>
   <si>
-    <t>51720,BETA US TEST,END USER BETA TEST US,9840751114,123 MAIN ST BUFFALO NY 14203 US,123@IM.COM</t>
-  </si>
-  <si>
-    <t>200,INGRAM MICRO TEST ACCOUNT,1610 E SAINT ANDREW PL ATTN TOD DEBIE SANTA ANA CA</t>
-  </si>
-  <si>
     <t>ModifyOrderLineDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>11,70,5</t>
+  </si>
+  <si>
+    <t>EP1234</t>
+  </si>
+  <si>
+    <t>RP1234</t>
+  </si>
+  <si>
+    <t>200,INGRAM MICRO TEST ACCOUNT,ATTN TOD DEBIE 1610 E SAINT ANDREW PL SANTA ANA CA</t>
+  </si>
+  <si>
+    <t>50067,IRFAN MEMON,Ingram Micro Test,0,1693 Alice Ct Annapolis MD 214016511 US,TEST@TEST.IM</t>
   </si>
 </sst>
 </file>
@@ -696,8 +705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
   <dimension ref="A1:AJ8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AK9" sqref="AK9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -841,7 +850,7 @@
         <v>63</v>
       </c>
       <c r="AJ1" s="7" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -985,7 +994,7 @@
         <v>27</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>69</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -1009,10 +1018,10 @@
         <v>49</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="Q6" t="s">
         <v>26</v>
@@ -1039,10 +1048,10 @@
         <v>29</v>
       </c>
       <c r="AF6" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="AG6" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:36" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added the code for OMS-3068, OMS-3073 and OMS-3059 stories
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86C0906-6F95-44CB-B6A3-3F4BE4DF1DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD0A6A4-F8FC-403F-8A03-467BB54196F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1575" yWindow="75" windowWidth="14745" windowHeight="10665" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="20040" windowHeight="10200" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -243,6 +243,9 @@
   </si>
   <si>
     <t>ModifyOrderLineDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>IM360DataErrorOrderConfirmationId</t>
   </si>
 </sst>
 </file>
@@ -694,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AK8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AK9" sqref="AK9"/>
+    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
+      <selection activeCell="AK11" sqref="AK11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,9 +735,10 @@
     <col min="34" max="34" width="36" customWidth="1"/>
     <col min="35" max="35" width="27.85546875" customWidth="1"/>
     <col min="36" max="36" width="31.42578125" customWidth="1"/>
+    <col min="37" max="37" width="33.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,8 +847,11 @@
       <c r="AJ1" s="7" t="s">
         <v>68</v>
       </c>
+      <c r="AK1" s="7" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="2" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -876,7 +883,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:36" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:37" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -950,7 +957,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
@@ -961,7 +968,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -971,7 +978,7 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>58</v>
       </c>
@@ -1045,11 +1052,11 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added the test cases for shipping Details, Shipping Address, Duplicate po for data error stories
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CD0A6A4-F8FC-403F-8A03-467BB54196F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC72122F-EAFD-4372-8F88-8C2161D046C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1170" yWindow="1170" windowWidth="20040" windowHeight="10200" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="73">
   <si>
     <t>FeatureFileName</t>
   </si>
@@ -140,9 +140,6 @@
     <t>FraudReprocessOrderConfirmationId</t>
   </si>
   <si>
-    <t>data_errors_orders</t>
-  </si>
-  <si>
     <t>DataErrorResubmitOrderConfirmationId</t>
   </si>
   <si>
@@ -246,6 +243,18 @@
   </si>
   <si>
     <t>IM360DataErrorOrderConfirmationId</t>
+  </si>
+  <si>
+    <t>X4DDataErrorOrderConfirmationId</t>
+  </si>
+  <si>
+    <t>ModifyShippingAddressDataErrorOrderID</t>
+  </si>
+  <si>
+    <t>order_exception_orders</t>
+  </si>
+  <si>
+    <t>X4CDuplicatePODataErrorOrderID</t>
   </si>
 </sst>
 </file>
@@ -697,15 +706,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
-  <dimension ref="A1:AK8"/>
+  <dimension ref="A1:AN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AF1" workbookViewId="0">
-      <selection activeCell="AK11" sqref="AK11"/>
+    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
+      <selection activeCell="AP5" sqref="AP5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
     <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
@@ -736,9 +745,12 @@
     <col min="35" max="35" width="27.85546875" customWidth="1"/>
     <col min="36" max="36" width="31.42578125" customWidth="1"/>
     <col min="37" max="37" width="33.5703125" customWidth="1"/>
+    <col min="38" max="38" width="33.7109375" customWidth="1"/>
+    <col min="39" max="39" width="44.28515625" customWidth="1"/>
+    <col min="40" max="40" width="32.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -803,55 +815,64 @@
         <v>33</v>
       </c>
       <c r="V1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="W1" s="7" t="s">
+      <c r="X1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="X1" s="7" t="s">
+      <c r="Y1" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="Y1" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="Z1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="7" t="s">
-        <v>43</v>
-      </c>
       <c r="AB1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="AC1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AC1" s="7" t="s">
+      <c r="AD1" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="AD1" s="7" t="s">
+      <c r="AE1" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="AE1" s="7" t="s">
-        <v>48</v>
-      </c>
       <c r="AF1" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG1" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="AG1" s="7" t="s">
-        <v>55</v>
-      </c>
       <c r="AH1" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI1" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AJ1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AL1" s="7" t="s">
         <v>69</v>
       </c>
+      <c r="AM1" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN1" s="7" t="s">
+        <v>72</v>
+      </c>
     </row>
-    <row r="2" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -859,19 +880,19 @@
         <v>20222222</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s">
         <v>28</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G2" s="11" t="s">
         <v>29</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -883,7 +904,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:37" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -891,7 +912,7 @@
         <v>20222222</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>27</v>
@@ -915,16 +936,16 @@
         <v>0</v>
       </c>
       <c r="M3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N3" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="P3" t="s">
         <v>49</v>
-      </c>
-      <c r="O3" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="P3" t="s">
-        <v>50</v>
       </c>
       <c r="Q3" t="s">
         <v>26</v>
@@ -936,13 +957,13 @@
         <v>24</v>
       </c>
       <c r="W3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X3" t="s">
         <v>39</v>
       </c>
-      <c r="X3" t="s">
+      <c r="Y3" t="s">
         <v>40</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>41</v>
       </c>
       <c r="Z3" t="s">
         <v>28</v>
@@ -951,26 +972,26 @@
         <v>29</v>
       </c>
       <c r="AF3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG3" t="s">
         <v>56</v>
       </c>
-      <c r="AG3" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="T4" t="s">
+        <v>51</v>
+      </c>
+      <c r="U4" t="s">
         <v>52</v>
       </c>
-      <c r="U4" t="s">
-        <v>53</v>
-      </c>
     </row>
-    <row r="5" spans="1:37" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>71</v>
       </c>
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
@@ -978,15 +999,15 @@
       <c r="H5" s="10"/>
       <c r="K5" s="10"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B6" s="4">
         <v>20222222</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" t="s">
         <v>27</v>
@@ -1010,16 +1031,16 @@
         <v>0</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="N6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="P6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q6" t="s">
         <v>26</v>
@@ -1031,13 +1052,13 @@
         <v>24</v>
       </c>
       <c r="W6" t="s">
+        <v>38</v>
+      </c>
+      <c r="X6" t="s">
         <v>39</v>
       </c>
-      <c r="X6" t="s">
+      <c r="Y6" t="s">
         <v>40</v>
-      </c>
-      <c r="Y6" t="s">
-        <v>41</v>
       </c>
       <c r="Z6" t="s">
         <v>28</v>
@@ -1046,17 +1067,17 @@
         <v>29</v>
       </c>
       <c r="AF6" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG6" t="s">
         <v>56</v>
       </c>
-      <c r="AG6" t="s">
-        <v>57</v>
-      </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B8" s="4"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sales order edit data modified
</commit_message>
<xml_diff>
--- a/TestData/Input_File.xlsx
+++ b/TestData/Input_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ussabd02\Documents\x4a-automation-test-suite\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uskrne00\Documents\x4a-automation-test-suite-neha\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC72122F-EAFD-4372-8F88-8C2161D046C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B06BDD4-C83D-4E49-9452-A0FEB25ABEC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="20040" windowHeight="10200" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{044CAF1B-95B2-4FAA-8E9D-FA372F0804C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_Data" sheetId="1" r:id="rId1"/>
@@ -233,12 +233,6 @@
     <t>20-VLJ7K-31</t>
   </si>
   <si>
-    <t>51720,BETA US TEST,END USER BETA TEST US,9840751114,123 MAIN ST BUFFALO NY 14203 US,123@IM.COM</t>
-  </si>
-  <si>
-    <t>200,INGRAM MICRO TEST ACCOUNT,1610 E SAINT ANDREW PL ATTN TOD DEBIE SANTA ANA CA</t>
-  </si>
-  <si>
     <t>ModifyOrderLineDataErrorOrderID</t>
   </si>
   <si>
@@ -255,6 +249,12 @@
   </si>
   <si>
     <t>X4CDuplicatePODataErrorOrderID</t>
+  </si>
+  <si>
+    <t>200,INGRAM MICRO TEST ACCOUNT,ATTN TOD DEBIE 1610 E SAINT ANDREW PL SANTA ANA CA 927054931,-,-,-</t>
+  </si>
+  <si>
+    <t>51291,APPLE,1700 E SAINT ANDREW PL Cash SANTA ANA CA 927054933 US,apple llc,9427135649,testing@ingrammicro.com</t>
   </si>
 </sst>
 </file>
@@ -708,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B262A89-DEBE-4ED1-96C9-9A0E865191D9}">
   <dimension ref="A1:AN8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AP5" sqref="AP5"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,19 +857,19 @@
         <v>62</v>
       </c>
       <c r="AJ1" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="AK1" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="AL1" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="AK1" s="7" t="s">
+      <c r="AM1" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="AL1" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="AM1" s="7" t="s">
+      <c r="AN1" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="AN1" s="7" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -991,7 +991,7 @@
     </row>
     <row r="5" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C5" s="9"/>
       <c r="F5" s="10"/>
@@ -1037,10 +1037,10 @@
         <v>48</v>
       </c>
       <c r="O6" s="8" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="Q6" t="s">
         <v>26</v>

</xml_diff>